<commit_message>
Fragen-Antwort Katalog updated. Update Anforderungsspezifikationen gemäss 2. Besprechung mit Hr. Lange.
</commit_message>
<xml_diff>
--- a/Projekt1/Fragen-Antworten-Katalog.xlsx
+++ b/Projekt1/Fragen-Antworten-Katalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yann/Documents/BFH Informatik/5 HS 2019/Projekt 1/bls/Projekt1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2BB71E-D955-D449-8E7B-D0117D315D3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD5DEA1-7A08-4E45-B040-0AFDA20B8CCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="24340" windowHeight="14980" xr2:uid="{C12555CE-3E7C-AA41-B5EE-8617F3E1DA16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Frage</t>
   </si>
@@ -126,7 +126,34 @@
     <t>closed</t>
   </si>
   <si>
-    <t>open</t>
+    <t>Zugservice/-komposition: muss eine Lokomotive in der Zugkomposition abgebildet werden?</t>
+  </si>
+  <si>
+    <t>Wie soll eine Strecke am besten mit An- &amp; Abfahrtszeiten abgebildet werden: Zeitangaben oder Dauerangaben (Dauerangaben ermöglichen eine schnellere Anpassung der Zeiten sowohl für die Erstellung der Zugservices wie auch bei Verspätungen)?</t>
+  </si>
+  <si>
+    <t>Sind Vorgaben für die Platznummerierung vorhangen (à la BLS)?</t>
+  </si>
+  <si>
+    <t>Soll die Applikation für z.B. 3 zu reservierende Plätze Vorschläge unterbreiten?</t>
+  </si>
+  <si>
+    <t>Besteht ein Wagen aus Abteilen? Oder ist diese Differenzierung nicht notwendig?</t>
+  </si>
+  <si>
+    <t>Nein, ist für die Sitzplatzreservation irrelevant</t>
+  </si>
+  <si>
+    <t>Dauerangaben bzw. Zeitintervalle.</t>
+  </si>
+  <si>
+    <t>Keine vorgesehen. Admin soll selber entscheiden können.</t>
+  </si>
+  <si>
+    <t>Gute Idee, verbesserte UX. Option!</t>
+  </si>
+  <si>
+    <t>Keine Abteile.</t>
   </si>
 </sst>
 </file>
@@ -519,11 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B6C229-211D-8D43-A068-06474D2DCE8B}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -547,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" hidden="1">
+    <row r="2" spans="1:4" ht="17">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -561,7 +587,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" hidden="1">
+    <row r="3" spans="1:4" ht="17">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -575,7 +601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" hidden="1">
+    <row r="4" spans="1:4" ht="17">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -589,7 +615,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28" hidden="1">
+    <row r="5" spans="1:4" ht="28">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -603,7 +629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34" hidden="1">
+    <row r="6" spans="1:4" ht="34">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -617,7 +643,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28" hidden="1">
+    <row r="7" spans="1:4" ht="28">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -631,7 +657,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="34" hidden="1">
+    <row r="8" spans="1:4" ht="34">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -645,7 +671,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17" hidden="1">
+    <row r="9" spans="1:4" ht="17">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -659,7 +685,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28" hidden="1">
+    <row r="10" spans="1:4" ht="28">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -673,7 +699,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="34" hidden="1">
+    <row r="11" spans="1:4" ht="34">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -687,7 +713,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28" hidden="1">
+    <row r="12" spans="1:4" ht="28">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -701,7 +727,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="42" hidden="1">
+    <row r="13" spans="1:4" ht="42">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -715,7 +741,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17" hidden="1">
+    <row r="14" spans="1:4" ht="17">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -729,7 +755,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17" hidden="1">
+    <row r="15" spans="1:4" ht="17">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -748,41 +774,70 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="17">
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="42">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="17">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="17">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17">
+      <c r="B20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D19" xr:uid="{2A8C3DA3-A55B-5B4C-8556-3DB3004FFF48}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="open"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D19" xr:uid="{2A8C3DA3-A55B-5B4C-8556-3DB3004FFF48}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>